<commit_message>
added player equip item
</commit_message>
<xml_diff>
--- a/Assets/Resources/ItemData/Randomize/ArtifactRandomizeByLevel.xlsx
+++ b/Assets/Resources/ItemData/Randomize/ArtifactRandomizeByLevel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PSG\Desktop\Capstone-Design-Project\Assets\Resources\ItemData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PSG\Desktop\Capstone-Design-Project\Assets\Resources\ItemData\Randomize\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F6963E-F04C-4B68-BCC1-7DF561203580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005CB0C0-6E57-41EE-BD7C-FD482B0ED579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="732" windowWidth="19332" windowHeight="11172" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="780" windowWidth="15624" windowHeight="11172" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Artifact" sheetId="1" r:id="rId1"/>
@@ -372,7 +372,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -396,7 +396,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>20</v>
@@ -413,10 +413,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C3">
         <v>0.2</v>
@@ -430,16 +430,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B4">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="C4">
         <v>0.3</v>
       </c>
       <c r="D4">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E4">
         <v>30</v>
@@ -447,16 +447,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B5">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="C5">
         <v>0.4</v>
       </c>
       <c r="D5">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="E5">
         <v>40</v>
@@ -464,16 +464,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B6">
-        <v>100</v>
+        <v>160</v>
       </c>
       <c r="C6">
         <v>0.5</v>
       </c>
       <c r="D6">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="E6">
         <v>50</v>
@@ -481,16 +481,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B7">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="C7">
         <v>0.6</v>
       </c>
       <c r="D7">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="E7">
         <v>60</v>
@@ -498,16 +498,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="B8">
-        <v>140</v>
+        <v>250</v>
       </c>
       <c r="C8">
         <v>0.7</v>
       </c>
       <c r="D8">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="E8">
         <v>70</v>
@@ -515,16 +515,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="B9">
-        <v>160</v>
+        <v>300</v>
       </c>
       <c r="C9">
         <v>0.8</v>
       </c>
       <c r="D9">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="E9">
         <v>80</v>
@@ -532,16 +532,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="B10">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="C10">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="E10">
         <v>90</v>

</xml_diff>

<commit_message>
item added crit options
</commit_message>
<xml_diff>
--- a/Assets/Resources/ItemData/Randomize/ArtifactRandomizeByLevel.xlsx
+++ b/Assets/Resources/ItemData/Randomize/ArtifactRandomizeByLevel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PSG\Desktop\Capstone-Design-Project\Assets\Resources\ItemData\Randomize\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005CB0C0-6E57-41EE-BD7C-FD482B0ED579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA9CB88-5228-4EC1-B271-E357A407904F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="780" windowWidth="15624" windowHeight="11172" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>DEF</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -44,6 +44,10 @@
   </si>
   <si>
     <t>ATK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CRIT_RATE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -369,15 +373,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -393,8 +397,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>5</v>
       </c>
@@ -410,8 +417,11 @@
       <c r="E2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>10</v>
       </c>
@@ -427,8 +437,11 @@
       <c r="E3">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>15</v>
       </c>
@@ -444,8 +457,11 @@
       <c r="E4">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>20</v>
       </c>
@@ -461,8 +477,11 @@
       <c r="E5">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>25</v>
       </c>
@@ -478,8 +497,11 @@
       <c r="E6">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>35</v>
       </c>
@@ -495,8 +517,11 @@
       <c r="E7">
         <v>60</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>45</v>
       </c>
@@ -512,8 +537,11 @@
       <c r="E8">
         <v>70</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>55</v>
       </c>
@@ -529,8 +557,11 @@
       <c r="E9">
         <v>80</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>65</v>
       </c>
@@ -545,6 +576,9 @@
       </c>
       <c r="E10">
         <v>90</v>
+      </c>
+      <c r="F10">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>